<commit_message>
tests: updated tests for new data outputs. Also changelog and compatibility warning
</commit_message>
<xml_diff>
--- a/psychopy/tests/test_data/corrXlsx.xlsx
+++ b/psychopy/tests/test_data/corrXlsx.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="420" windowWidth="21600" windowHeight="13320"/>
+    <workbookView xWindow="240" yWindow="6040" windowWidth="21600" windowHeight="13320"/>
   </bookViews>
   <sheets>
     <sheet name="rawData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>rt_mean</t>
   </si>
@@ -39,16 +39,31 @@
     <t>resp_std</t>
   </si>
   <si>
-    <t>index_mean</t>
-  </si>
-  <si>
-    <t>index_raw</t>
-  </si>
-  <si>
-    <t>index_std</t>
-  </si>
-  <si>
     <t>rt_std</t>
+  </si>
+  <si>
+    <t>congruent</t>
+  </si>
+  <si>
+    <t>corrAns</t>
+  </si>
+  <si>
+    <t>letterColor</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
@@ -88,8 +103,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,27 +400,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -422,24 +440,27 @@
         <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>6.5</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>3.5355339059299999</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -465,26 +486,33 @@
       <c r="M2">
         <v>0</v>
       </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
       <c r="E3">
-        <v>5.6568542494900003</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
+      <c r="G3" s="1"/>
       <c r="H3">
         <v>1</v>
       </c>
@@ -500,22 +528,28 @@
       <c r="M3">
         <v>0</v>
       </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>4.5</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>2.1213203435599999</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -541,22 +575,28 @@
       <c r="M4">
         <v>0.14142136361300001</v>
       </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>6.5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>2.1213203435599999</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>2.5</v>
@@ -582,22 +622,28 @@
       <c r="M5">
         <v>7.07106844407E-2</v>
       </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>5.5</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>7.7781745930500001</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -623,22 +669,28 @@
       <c r="M6">
         <v>0</v>
       </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
       </c>
       <c r="E7">
-        <v>4.2426406871199998</v>
+        <v>2</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -664,9 +716,14 @@
       <c r="M7">
         <v>0.14142136361300001</v>
       </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>